<commit_message>
Miglioramenti grafici, implementazione dei caricamenti da file
</commit_message>
<xml_diff>
--- a/pages/super_user/inserimento/docenti/Stage_Manager_Modulo_Docenti.xlsx
+++ b/pages/super_user/inserimento/docenti/Stage_Manager_Modulo_Docenti.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -115,7 +115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -132,17 +132,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -154,6 +148,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -502,14 +499,14 @@
   <dimension ref="A1:AP1165"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:B2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" style="8" customWidth="1"/>
     <col min="4" max="4" width="29.5703125" style="3" customWidth="1"/>
     <col min="7" max="30" width="18.28515625" style="1" customWidth="1"/>
     <col min="31" max="42" width="9.140625" style="1"/>
@@ -522,7 +519,7 @@
       <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -530,575 +527,575 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="11"/>
+      <c r="A2" s="12"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="11"/>
+      <c r="A3" s="12"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="11"/>
-      <c r="H4" s="12" t="s">
+      <c r="A4" s="12"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="9"/>
+      <c r="H4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="11"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
+      <c r="A5" s="12"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="9"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="11"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
+      <c r="A6" s="12"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="9"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="11"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
+      <c r="A7" s="12"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="9"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="11"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
+      <c r="A8" s="12"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="9"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="11"/>
+      <c r="A9" s="12"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="11"/>
-      <c r="H10" s="13" t="s">
+      <c r="A10" s="12"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="9"/>
+      <c r="H10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="11"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
+      <c r="A11" s="12"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="9"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="11"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
+      <c r="A12" s="12"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="9"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="11"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
+      <c r="A13" s="12"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="9"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="11"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
+      <c r="A14" s="12"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="9"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="6"/>
+      <c r="A15" s="12"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="12"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="6"/>
+      <c r="A16" s="12"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="12"/>
     </row>
     <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="6"/>
+      <c r="A17" s="12"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="12"/>
     </row>
     <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="6"/>
+      <c r="A18" s="12"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="12"/>
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+      <c r="A19" s="12"/>
     </row>
     <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+      <c r="A20" s="12"/>
     </row>
     <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
+      <c r="A21" s="12"/>
     </row>
     <row r="22" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
+      <c r="A22" s="12"/>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+      <c r="A23" s="12"/>
     </row>
     <row r="24" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="D24" s="11"/>
+      <c r="A24" s="12"/>
+      <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="D25" s="11"/>
+      <c r="A25" s="12"/>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="D26" s="11"/>
+      <c r="A26" s="12"/>
+      <c r="D26" s="9"/>
     </row>
     <row r="27" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="D27" s="11"/>
+      <c r="A27" s="12"/>
+      <c r="D27" s="9"/>
     </row>
     <row r="28" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="D28" s="11"/>
+      <c r="A28" s="12"/>
+      <c r="D28" s="9"/>
     </row>
     <row r="29" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="D29" s="11"/>
+      <c r="A29" s="12"/>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="D30" s="11"/>
+      <c r="A30" s="12"/>
+      <c r="D30" s="9"/>
     </row>
     <row r="31" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
+      <c r="A31" s="12"/>
     </row>
     <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="C32" s="8"/>
+      <c r="A32" s="12"/>
+      <c r="C32" s="7"/>
     </row>
     <row r="33" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="C33" s="8"/>
+      <c r="A33" s="12"/>
+      <c r="C33" s="7"/>
     </row>
     <row r="34" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="C34" s="8"/>
+      <c r="A34" s="12"/>
+      <c r="C34" s="7"/>
     </row>
     <row r="35" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="C35" s="8"/>
+      <c r="A35" s="12"/>
+      <c r="C35" s="7"/>
     </row>
     <row r="36" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="D36" s="11"/>
+      <c r="A36" s="12"/>
+      <c r="D36" s="9"/>
     </row>
     <row r="37" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="D37" s="11"/>
+      <c r="A37" s="12"/>
+      <c r="D37" s="9"/>
     </row>
     <row r="38" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="D38" s="11"/>
+      <c r="A38" s="12"/>
+      <c r="D38" s="9"/>
     </row>
     <row r="39" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="D39" s="11"/>
+      <c r="A39" s="12"/>
+      <c r="D39" s="9"/>
     </row>
     <row r="40" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="D40" s="11"/>
+      <c r="A40" s="12"/>
+      <c r="D40" s="9"/>
     </row>
     <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="D41" s="11"/>
+      <c r="A41" s="12"/>
+      <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="D42" s="11"/>
+      <c r="A42" s="12"/>
+      <c r="D42" s="9"/>
     </row>
     <row r="43" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="D43" s="11"/>
+      <c r="A43" s="12"/>
+      <c r="D43" s="9"/>
     </row>
     <row r="44" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
+      <c r="A44" s="12"/>
     </row>
     <row r="45" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
+      <c r="A45" s="12"/>
     </row>
     <row r="46" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
+      <c r="A46" s="12"/>
     </row>
     <row r="47" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
+      <c r="A47" s="12"/>
     </row>
     <row r="48" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
+      <c r="A48" s="12"/>
     </row>
     <row r="49" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
+      <c r="A49" s="12"/>
     </row>
     <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
+      <c r="A50" s="12"/>
     </row>
     <row r="51" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
+      <c r="A51" s="12"/>
     </row>
     <row r="52" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
+      <c r="A52" s="12"/>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
+      <c r="A53" s="12"/>
     </row>
     <row r="54" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
+      <c r="A54" s="12"/>
     </row>
     <row r="55" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
-      <c r="C55" s="8"/>
+      <c r="A55" s="12"/>
+      <c r="C55" s="7"/>
     </row>
     <row r="56" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
-      <c r="C56" s="8"/>
+      <c r="A56" s="12"/>
+      <c r="C56" s="7"/>
     </row>
     <row r="57" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
-      <c r="C57" s="8"/>
+      <c r="A57" s="12"/>
+      <c r="C57" s="7"/>
     </row>
     <row r="58" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
-      <c r="C58" s="8"/>
+      <c r="A58" s="12"/>
+      <c r="C58" s="7"/>
     </row>
     <row r="59" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="6"/>
+      <c r="A59" s="12"/>
     </row>
     <row r="60" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="6"/>
+      <c r="A60" s="12"/>
     </row>
     <row r="61" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="6"/>
-      <c r="D61" s="11"/>
+      <c r="A61" s="12"/>
+      <c r="D61" s="9"/>
     </row>
     <row r="62" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="6"/>
-      <c r="D62" s="11"/>
+      <c r="A62" s="12"/>
+      <c r="D62" s="9"/>
     </row>
     <row r="63" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="6"/>
-      <c r="D63" s="11"/>
+      <c r="A63" s="12"/>
+      <c r="D63" s="9"/>
     </row>
     <row r="64" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
-      <c r="D64" s="11"/>
+      <c r="A64" s="12"/>
+      <c r="D64" s="9"/>
     </row>
     <row r="65" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="6"/>
-      <c r="D65" s="11"/>
+      <c r="A65" s="12"/>
+      <c r="D65" s="9"/>
     </row>
     <row r="66" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
+      <c r="A66" s="12"/>
     </row>
     <row r="67" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
-      <c r="C67" s="8"/>
+      <c r="A67" s="12"/>
+      <c r="C67" s="7"/>
     </row>
     <row r="68" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="6"/>
-      <c r="C68" s="8"/>
+      <c r="A68" s="12"/>
+      <c r="C68" s="7"/>
     </row>
     <row r="69" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="6"/>
-      <c r="C69" s="8"/>
+      <c r="A69" s="12"/>
+      <c r="C69" s="7"/>
     </row>
     <row r="70" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
-      <c r="C70" s="8"/>
+      <c r="A70" s="12"/>
+      <c r="C70" s="7"/>
     </row>
     <row r="71" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="6"/>
+      <c r="A71" s="12"/>
     </row>
     <row r="72" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="6"/>
+      <c r="A72" s="12"/>
     </row>
     <row r="73" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="6"/>
+      <c r="A73" s="12"/>
     </row>
     <row r="74" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="6"/>
-      <c r="D74" s="11"/>
+      <c r="A74" s="12"/>
+      <c r="D74" s="9"/>
     </row>
     <row r="75" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="6"/>
-      <c r="D75" s="11"/>
+      <c r="A75" s="12"/>
+      <c r="D75" s="9"/>
     </row>
     <row r="76" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="6"/>
-      <c r="D76" s="11"/>
+      <c r="A76" s="12"/>
+      <c r="D76" s="9"/>
     </row>
     <row r="77" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="6"/>
-      <c r="D77" s="11"/>
+      <c r="A77" s="12"/>
+      <c r="D77" s="9"/>
     </row>
     <row r="78" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="6"/>
-      <c r="D78" s="11"/>
+      <c r="A78" s="12"/>
+      <c r="D78" s="9"/>
     </row>
     <row r="79" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="6"/>
-      <c r="D79" s="11"/>
+      <c r="A79" s="12"/>
+      <c r="D79" s="9"/>
     </row>
     <row r="80" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="6"/>
-      <c r="D80" s="11"/>
+      <c r="A80" s="12"/>
+      <c r="D80" s="9"/>
     </row>
     <row r="81" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="6"/>
-      <c r="D81" s="11"/>
+      <c r="A81" s="12"/>
+      <c r="D81" s="9"/>
     </row>
     <row r="82" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="6"/>
+      <c r="A82" s="12"/>
     </row>
     <row r="83" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="6"/>
+      <c r="A83" s="12"/>
     </row>
     <row r="84" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="6"/>
+      <c r="A84" s="12"/>
     </row>
     <row r="85" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="6"/>
+      <c r="A85" s="12"/>
     </row>
     <row r="86" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="6"/>
+      <c r="A86" s="12"/>
     </row>
     <row r="87" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="6"/>
+      <c r="A87" s="12"/>
     </row>
     <row r="88" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="6"/>
-      <c r="C88" s="8"/>
+      <c r="A88" s="12"/>
+      <c r="C88" s="7"/>
     </row>
     <row r="89" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="6"/>
-      <c r="C89" s="8"/>
+      <c r="A89" s="12"/>
+      <c r="C89" s="7"/>
     </row>
     <row r="90" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="6"/>
-      <c r="C90" s="8"/>
+      <c r="A90" s="12"/>
+      <c r="C90" s="7"/>
     </row>
     <row r="91" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="6"/>
-      <c r="C91" s="8"/>
+      <c r="A91" s="12"/>
+      <c r="C91" s="7"/>
     </row>
     <row r="92" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="6"/>
+      <c r="A92" s="12"/>
     </row>
     <row r="93" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="6"/>
-      <c r="D93" s="11"/>
+      <c r="A93" s="12"/>
+      <c r="D93" s="9"/>
     </row>
     <row r="94" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="6"/>
-      <c r="D94" s="11"/>
+      <c r="A94" s="12"/>
+      <c r="D94" s="9"/>
     </row>
     <row r="95" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="6"/>
-      <c r="D95" s="11"/>
+      <c r="A95" s="12"/>
+      <c r="D95" s="9"/>
     </row>
     <row r="96" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="6"/>
-      <c r="D96" s="11"/>
+      <c r="A96" s="12"/>
+      <c r="D96" s="9"/>
     </row>
     <row r="97" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="6"/>
-      <c r="D97" s="11"/>
+      <c r="A97" s="12"/>
+      <c r="D97" s="9"/>
     </row>
     <row r="98" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="6"/>
-      <c r="D98" s="11"/>
+      <c r="A98" s="12"/>
+      <c r="D98" s="9"/>
     </row>
     <row r="99" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="6"/>
+      <c r="A99" s="12"/>
     </row>
     <row r="100" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="6"/>
-      <c r="C100" s="8"/>
+      <c r="A100" s="12"/>
+      <c r="C100" s="7"/>
     </row>
     <row r="101" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="6"/>
-      <c r="C101" s="8"/>
+      <c r="A101" s="12"/>
+      <c r="C101" s="7"/>
     </row>
     <row r="102" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="6"/>
-      <c r="C102" s="8"/>
+      <c r="A102" s="12"/>
+      <c r="C102" s="7"/>
     </row>
     <row r="103" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="6"/>
-      <c r="C103" s="8"/>
+      <c r="A103" s="12"/>
+      <c r="C103" s="7"/>
     </row>
     <row r="104" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="6"/>
+      <c r="A104" s="12"/>
     </row>
     <row r="105" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="6"/>
+      <c r="A105" s="12"/>
     </row>
     <row r="106" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="6"/>
+      <c r="A106" s="12"/>
     </row>
     <row r="107" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="6"/>
-      <c r="D107" s="11"/>
+      <c r="A107" s="12"/>
+      <c r="D107" s="9"/>
     </row>
     <row r="108" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="6"/>
-      <c r="D108" s="11"/>
+      <c r="A108" s="12"/>
+      <c r="D108" s="9"/>
     </row>
     <row r="109" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="6"/>
-      <c r="D109" s="11"/>
+      <c r="A109" s="12"/>
+      <c r="D109" s="9"/>
     </row>
     <row r="110" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="6"/>
-      <c r="D110" s="11"/>
+      <c r="A110" s="12"/>
+      <c r="D110" s="9"/>
     </row>
     <row r="111" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="6"/>
-      <c r="D111" s="11"/>
+      <c r="A111" s="12"/>
+      <c r="D111" s="9"/>
     </row>
     <row r="112" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="6"/>
-      <c r="D112" s="11"/>
+      <c r="A112" s="12"/>
+      <c r="D112" s="9"/>
     </row>
     <row r="113" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="6"/>
-      <c r="D113" s="11"/>
+      <c r="A113" s="12"/>
+      <c r="D113" s="9"/>
     </row>
     <row r="114" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="6"/>
-      <c r="D114" s="11"/>
+      <c r="A114" s="12"/>
+      <c r="D114" s="9"/>
     </row>
     <row r="115" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="6"/>
+      <c r="A115" s="12"/>
     </row>
     <row r="116" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="6"/>
+      <c r="A116" s="12"/>
     </row>
     <row r="117" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="6"/>
-      <c r="C117" s="8"/>
+      <c r="A117" s="12"/>
+      <c r="C117" s="7"/>
     </row>
     <row r="118" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="6"/>
-      <c r="C118" s="8"/>
+      <c r="A118" s="12"/>
+      <c r="C118" s="7"/>
     </row>
     <row r="119" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="6"/>
-      <c r="C119" s="8"/>
+      <c r="A119" s="12"/>
+      <c r="C119" s="7"/>
     </row>
     <row r="120" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="6"/>
-      <c r="C120" s="8"/>
+      <c r="A120" s="12"/>
+      <c r="C120" s="7"/>
     </row>
     <row r="121" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="6"/>
+      <c r="A121" s="12"/>
     </row>
     <row r="122" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="6"/>
+      <c r="A122" s="12"/>
     </row>
     <row r="123" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="6"/>
-      <c r="D123" s="11"/>
+      <c r="A123" s="12"/>
+      <c r="D123" s="9"/>
     </row>
     <row r="124" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="6"/>
-      <c r="D124" s="11"/>
+      <c r="A124" s="12"/>
+      <c r="D124" s="9"/>
     </row>
     <row r="125" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="6"/>
-      <c r="D125" s="11"/>
+      <c r="A125" s="12"/>
+      <c r="D125" s="9"/>
     </row>
     <row r="126" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="6"/>
-      <c r="D126" s="11"/>
+      <c r="A126" s="12"/>
+      <c r="D126" s="9"/>
     </row>
     <row r="127" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="6"/>
-      <c r="D127" s="11"/>
+      <c r="A127" s="12"/>
+      <c r="D127" s="9"/>
     </row>
     <row r="128" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="6"/>
-      <c r="D128" s="11"/>
+      <c r="A128" s="12"/>
+      <c r="D128" s="9"/>
     </row>
     <row r="129" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="6"/>
-      <c r="D129" s="11"/>
+      <c r="A129" s="12"/>
+      <c r="D129" s="9"/>
     </row>
     <row r="130" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="6"/>
-      <c r="D130" s="11"/>
+      <c r="A130" s="12"/>
+      <c r="D130" s="9"/>
     </row>
     <row r="131" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="6"/>
-      <c r="D131" s="11"/>
+      <c r="A131" s="12"/>
+      <c r="D131" s="9"/>
     </row>
     <row r="132" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="6"/>
+      <c r="A132" s="12"/>
     </row>
     <row r="133" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="6"/>
+      <c r="A133" s="12"/>
     </row>
     <row r="134" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="6"/>
+      <c r="A134" s="12"/>
     </row>
     <row r="135" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="6"/>
+      <c r="A135" s="12"/>
     </row>
     <row r="136" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="6"/>
+      <c r="A136" s="12"/>
     </row>
     <row r="137" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="6"/>
+      <c r="A137" s="12"/>
     </row>
     <row r="138" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="139" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>